<commit_message>
changes in stats page
</commit_message>
<xml_diff>
--- a/src/file_format/stat_format.xlsx
+++ b/src/file_format/stat_format.xlsx
@@ -21,35 +21,35 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Student Id</t>
-  </si>
-  <si>
-    <t>branch</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>s.no</t>
-  </si>
-  <si>
-    <t>student name</t>
-  </si>
-  <si>
-    <t>phone number</t>
-  </si>
-  <si>
-    <t>company name</t>
-  </si>
-  <si>
-    <t>role</t>
+    <t>rollNo</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Salary Offered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -60,6 +60,23 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -83,9 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -304,166 +323,157 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
   </sheetData>

</xml_diff>